<commit_message>
update api table- 2
</commit_message>
<xml_diff>
--- a/server/api.xlsx
+++ b/server/api.xlsx
@@ -1,36 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guy Levi\Desktop\Bunniez\server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/moriaor/Google Drive/moria.or/year3/semester_b/postpc-final/Bunniez/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12B30822-C3AE-4C29-9B35-3F069BBD4E5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00150ABB-1C70-B645-ADB5-0A009F74955A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="3795" windowWidth="28800" windowHeight="15885" xr2:uid="{EB39B21D-63FA-4507-B5A7-45EC560A1FFF}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="15880" xr2:uid="{EB39B21D-63FA-4507-B5A7-45EC560A1FFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>index</t>
   </si>
@@ -104,9 +99,6 @@
     <t>chosen indexes</t>
   </si>
   <si>
-    <t>final</t>
-  </si>
-  <si>
     <t>final.jpg</t>
   </si>
   <si>
@@ -119,12 +111,6 @@
     <t>initiate preprocessing, save to output directory</t>
   </si>
   <si>
-    <t>initiate processing, save as final.jpg to output directory</t>
-  </si>
-  <si>
-    <t>send file final.jpg from output directory</t>
-  </si>
-  <si>
     <t>delete root directory, delete util object</t>
   </si>
   <si>
@@ -132,6 +118,9 @@
   </si>
   <si>
     <t>GET</t>
+  </si>
+  <si>
+    <t>initiate processing, save as final.jpg to output directory and send file final.jpg from output directory</t>
   </si>
 </sst>
 </file>
@@ -225,11 +214,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,76 +533,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E48191B0-1A99-4A30-86F1-CD0B1075E784}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="157" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="6" width="9.140625" style="2"/>
-    <col min="7" max="7" width="9.140625" style="3"/>
-    <col min="8" max="10" width="9.140625" style="2"/>
-    <col min="11" max="11" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.1640625" style="4"/>
+    <col min="2" max="3" width="9.1640625" style="2"/>
+    <col min="4" max="4" width="9.1640625" style="1"/>
+    <col min="5" max="6" width="9.1640625" style="2"/>
+    <col min="7" max="7" width="9.1640625" style="3"/>
+    <col min="8" max="10" width="9.1640625" style="2"/>
+    <col min="11" max="11" width="9.1640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
+      <c r="E2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="I2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>0</v>
       </c>
@@ -635,11 +624,11 @@
       <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>32</v>
+      <c r="L3" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -670,11 +659,11 @@
       <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>26</v>
+      <c r="L4" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -687,154 +676,122 @@
       <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="8" t="s">
+      <c r="I5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="8" t="s">
-        <v>28</v>
+      <c r="L5" s="7" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>33</v>
+      <c r="C6" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="8" t="s">
+      <c r="I6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>16</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="8" t="s">
-        <v>27</v>
+      <c r="L6" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L7" s="8" t="s">
-        <v>29</v>
+      <c r="K7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>33</v>
+      <c r="C8" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>24</v>
+        <v>20</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>31</v>
+      <c r="L8" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated server API spreadsheet and server directory cleanup
</commit_message>
<xml_diff>
--- a/server/api.xlsx
+++ b/server/api.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guy Levi\Desktop\Bunniez\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91033633-92B5-479B-A4E7-1F0254E18D12}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37F6E4C-DDD3-4D01-B27D-2EFFF0D37086}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="3795" windowWidth="28800" windowHeight="15885" xr2:uid="{EB39B21D-63FA-4507-B5A7-45EC560A1FFF}"/>
+    <workbookView xWindow="12225" yWindow="2040" windowWidth="24630" windowHeight="12405" xr2:uid="{EB39B21D-63FA-4507-B5A7-45EC560A1FFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>POST</t>
-  </si>
-  <si>
     <t>init</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>save file as index.jpg in input directory, add to imutils</t>
+  </si>
+  <si>
+    <t>HEAD</t>
   </si>
 </sst>
 </file>
@@ -207,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -219,6 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +537,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,43 +609,43 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="9">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>4</v>
@@ -653,65 +654,65 @@
         <v>0</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="L4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="9">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
+      <c r="C5" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="L5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="9">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>4</v>
@@ -720,83 +721,83 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="9">
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="L7" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="9">
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>